<commit_message>
reordering table 1 countries
</commit_message>
<xml_diff>
--- a/tables/Table1.xlsx
+++ b/tables/Table1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissoria/Documents/Research/us_international_ses/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA598F90-1C80-204A-96BA-87BE9594E6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5A4926-8AC5-8742-BEDC-6B5EE0CAB203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49840" yWindow="-1780" windowWidth="27300" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="4980" windowWidth="25120" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Country</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Percent of Migrants</t>
   </si>
   <si>
-    <t>GDP</t>
-  </si>
-  <si>
     <t>Life Expectancy at 60</t>
   </si>
   <si>
@@ -46,75 +43,78 @@
     <t>Mexico and Carribean Countries</t>
   </si>
   <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Central American Countries</t>
+  </si>
+  <si>
+    <t>Belize/British Honduras</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>South American Countries</t>
+  </si>
+  <si>
     <t>Argentina</t>
   </si>
   <si>
-    <t>Belize/British Honduras</t>
-  </si>
-  <si>
     <t>Bolivia</t>
   </si>
   <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>Chile</t>
   </si>
   <si>
     <t>Colombia</t>
   </si>
   <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>Cuba</t>
-  </si>
-  <si>
-    <t>Dominican Republic</t>
-  </si>
-  <si>
     <t>Ecuador</t>
   </si>
   <si>
-    <t>El Salvador</t>
-  </si>
-  <si>
-    <t>Guatemala</t>
-  </si>
-  <si>
     <t>Guyana/British Guiana</t>
   </si>
   <si>
     <t>Haiti</t>
   </si>
   <si>
-    <t>Honduras</t>
-  </si>
-  <si>
     <t>Jamaica</t>
   </si>
   <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Nicaragua</t>
-  </si>
-  <si>
-    <t>Panama</t>
-  </si>
-  <si>
     <t>Paraguay</t>
   </si>
   <si>
     <t>Peru</t>
   </si>
   <si>
-    <t>Puerto Rico</t>
-  </si>
-  <si>
     <t>Trinidad and Tobago</t>
   </si>
   <si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Venezuela</t>
+  </si>
+  <si>
+    <t>GDP Per Capita</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,7 +488,7 @@
     <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -501,618 +504,605 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>48615</v>
+        <v>1809510</v>
       </c>
       <c r="C3">
-        <v>1.1817698999999999</v>
+        <v>43.986924999999999</v>
       </c>
       <c r="D3">
-        <v>14187.5</v>
+        <v>13790</v>
       </c>
       <c r="E3">
-        <v>21.59</v>
+        <v>22.200001</v>
       </c>
       <c r="F3">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="G3">
-        <v>7.7482425089999998</v>
+        <v>10.78765175</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>1912</v>
+        <v>462503</v>
       </c>
       <c r="C4">
-        <v>4.64783E-2</v>
+        <v>11.24287</v>
       </c>
       <c r="D4">
-        <v>7460</v>
+        <v>9605.2999999999993</v>
       </c>
       <c r="E4">
-        <v>21.690000999999999</v>
+        <v>21.57</v>
       </c>
       <c r="F4">
-        <v>89.337112000000005</v>
+        <v>87.121002000000004</v>
       </c>
       <c r="G4">
-        <v>12.42360178</v>
+        <v>4.8892123959999996</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>16749</v>
+        <v>248511</v>
       </c>
       <c r="C5">
-        <v>0.40714729999999999</v>
+        <v>6.0409917999999996</v>
       </c>
       <c r="D5">
-        <v>3686.3</v>
+        <v>10717.6</v>
       </c>
       <c r="E5">
-        <v>19.420000000000002</v>
+        <v>22.6</v>
       </c>
       <c r="F5">
-        <v>182.161</v>
+        <v>63</v>
       </c>
       <c r="G5">
-        <v>28.826000000000001</v>
+        <v>4.1387709199999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>7814</v>
+        <v>540375</v>
       </c>
       <c r="C6">
-        <v>0.1899486</v>
+        <v>13.135840999999999</v>
       </c>
       <c r="D6">
-        <v>10294.9</v>
+        <v>36779.1</v>
       </c>
       <c r="E6">
-        <v>21.32</v>
+        <v>25.32</v>
       </c>
       <c r="F6">
-        <v>143.76801</v>
+        <v>70.530997999999997</v>
       </c>
       <c r="G6">
-        <v>11.8134596</v>
+        <v>5.3090000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>2922</v>
-      </c>
-      <c r="C7">
-        <v>7.1030200000000002E-2</v>
-      </c>
-      <c r="D7">
-        <v>53431.199999999997</v>
-      </c>
-      <c r="E7">
-        <v>24.99</v>
-      </c>
-      <c r="F7">
-        <v>41.473202000000001</v>
-      </c>
-      <c r="G7">
-        <v>4.4358505600000004</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>27920</v>
+        <v>1912</v>
       </c>
       <c r="C8">
-        <v>0.67870030000000003</v>
+        <v>4.64783E-2</v>
       </c>
       <c r="D8">
-        <v>17067.8</v>
+        <v>7460</v>
       </c>
       <c r="E8">
-        <v>24.57</v>
+        <v>21.690000999999999</v>
       </c>
       <c r="F8">
-        <v>139</v>
+        <v>89.337112000000005</v>
       </c>
       <c r="G8">
-        <v>6.5529999999999999</v>
+        <v>12.42360178</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>194022</v>
+        <v>20884</v>
       </c>
       <c r="C9">
-        <v>4.7164324999999998</v>
+        <v>0.50766389999999995</v>
       </c>
       <c r="D9">
-        <v>6947.4</v>
+        <v>16942</v>
       </c>
       <c r="E9">
-        <v>22.690000999999999</v>
+        <v>24.52</v>
       </c>
       <c r="F9">
-        <v>97.325325000000007</v>
+        <v>80.935242000000002</v>
       </c>
       <c r="G9">
-        <v>9.3586532479999995</v>
+        <v>7.2910775140000004</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>20884</v>
+        <v>198955</v>
       </c>
       <c r="C10">
-        <v>0.50766389999999995</v>
+        <v>4.8363472999999999</v>
       </c>
       <c r="D10">
-        <v>16942</v>
+        <v>5391.1</v>
       </c>
       <c r="E10">
-        <v>24.52</v>
+        <v>22.01</v>
       </c>
       <c r="F10">
-        <v>80.935242000000002</v>
+        <v>78.046379000000002</v>
       </c>
       <c r="G10">
-        <v>7.2910775140000004</v>
+        <v>14.05</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>462503</v>
+        <v>99842</v>
       </c>
       <c r="C11">
-        <v>11.24287</v>
+        <v>2.4270342999999999</v>
       </c>
       <c r="D11">
-        <v>9605.2999999999993</v>
+        <v>5762.8</v>
       </c>
       <c r="E11">
-        <v>21.57</v>
+        <v>20.65</v>
       </c>
       <c r="F11">
-        <v>87.121002000000004</v>
+        <v>107</v>
       </c>
       <c r="G11">
-        <v>4.8892123959999996</v>
+        <v>18.537905510000002</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>248511</v>
+        <v>60125</v>
       </c>
       <c r="C12">
-        <v>6.0409917999999996</v>
+        <v>1.4615636000000001</v>
       </c>
       <c r="D12">
-        <v>10717.6</v>
+        <v>3231.7</v>
       </c>
       <c r="E12">
-        <v>22.6</v>
+        <v>18.129999000000002</v>
       </c>
       <c r="F12">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="G12">
-        <v>4.1387709199999998</v>
+        <v>14.656000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>91850</v>
+        <v>60186</v>
       </c>
       <c r="C13">
-        <v>2.2327587000000002</v>
+        <v>1.4630464999999999</v>
       </c>
       <c r="D13">
-        <v>6609.8</v>
+        <v>2612.9</v>
       </c>
       <c r="E13">
-        <v>22.83</v>
+        <v>24.5</v>
       </c>
       <c r="F13">
-        <v>144.01900000000001</v>
+        <v>55.144607999999998</v>
       </c>
       <c r="G13">
-        <v>10.15329704</v>
+        <v>12.590981080000001</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14">
-        <v>198955</v>
+        <v>33245</v>
       </c>
       <c r="C14">
-        <v>4.8363472999999999</v>
+        <v>0.80814439999999998</v>
       </c>
       <c r="D14">
-        <v>5391.1</v>
+        <v>18686.400000000001</v>
       </c>
       <c r="E14">
-        <v>22.01</v>
+        <v>23.98</v>
       </c>
       <c r="F14">
-        <v>78.046379000000002</v>
+        <v>53.020954000000003</v>
       </c>
       <c r="G14">
-        <v>14.05</v>
+        <v>14.27296808</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>99842</v>
-      </c>
-      <c r="C15">
-        <v>2.4270342999999999</v>
-      </c>
-      <c r="D15">
-        <v>5762.8</v>
-      </c>
-      <c r="E15">
-        <v>20.65</v>
-      </c>
-      <c r="F15">
-        <v>107</v>
-      </c>
-      <c r="G15">
-        <v>18.537905510000002</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>2234</v>
+        <v>48615</v>
       </c>
       <c r="C16">
-        <v>5.4305699999999998E-2</v>
+        <v>1.1817698999999999</v>
       </c>
       <c r="D16">
-        <v>20765.400000000001</v>
+        <v>14187.5</v>
       </c>
       <c r="E16">
-        <v>18.010000000000002</v>
+        <v>21.59</v>
       </c>
       <c r="F16">
-        <v>82.800003000000004</v>
+        <v>68</v>
       </c>
       <c r="G16">
-        <v>11.40276751</v>
+        <v>7.7482425089999998</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>1739</v>
+        <v>16749</v>
       </c>
       <c r="C17">
-        <v>4.2272900000000002E-2</v>
+        <v>0.40714729999999999</v>
       </c>
       <c r="D17">
-        <v>1705.8</v>
+        <v>3686.3</v>
       </c>
       <c r="E17">
-        <v>16.25</v>
+        <v>19.420000000000002</v>
       </c>
       <c r="F17">
-        <v>237.19299000000001</v>
+        <v>182.161</v>
       </c>
       <c r="G17">
-        <v>53.034999999999997</v>
+        <v>28.826000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>60125</v>
+        <v>7814</v>
       </c>
       <c r="C18">
-        <v>1.4615636000000001</v>
+        <v>0.1899486</v>
       </c>
       <c r="D18">
-        <v>3231.7</v>
+        <v>10294.9</v>
       </c>
       <c r="E18">
-        <v>18.129999000000002</v>
+        <v>21.32</v>
       </c>
       <c r="F18">
-        <v>86</v>
+        <v>143.76801</v>
       </c>
       <c r="G18">
-        <v>14.656000000000001</v>
+        <v>11.8134596</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
-        <v>2627</v>
+        <v>27920</v>
       </c>
       <c r="C19">
-        <v>6.3859100000000002E-2</v>
+        <v>0.67870030000000003</v>
       </c>
       <c r="D19">
-        <v>6839.7</v>
+        <v>17067.8</v>
       </c>
       <c r="E19">
-        <v>18.66</v>
+        <v>24.57</v>
       </c>
       <c r="F19">
-        <v>91.873001000000002</v>
+        <v>139</v>
       </c>
       <c r="G19">
-        <v>11.555999999999999</v>
+        <v>6.5529999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>1809510</v>
+        <v>194022</v>
       </c>
       <c r="C20">
-        <v>43.986924999999999</v>
+        <v>4.7164324999999998</v>
       </c>
       <c r="D20">
-        <v>13790</v>
+        <v>6947.4</v>
       </c>
       <c r="E20">
-        <v>22.200001</v>
+        <v>22.690000999999999</v>
       </c>
       <c r="F20">
-        <v>96</v>
+        <v>97.325325000000007</v>
       </c>
       <c r="G20">
-        <v>10.78765175</v>
+        <v>9.3586532479999995</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21">
-        <v>60186</v>
+        <v>91850</v>
       </c>
       <c r="C21">
-        <v>1.4630464999999999</v>
+        <v>2.2327587000000002</v>
       </c>
       <c r="D21">
-        <v>2612.9</v>
+        <v>6609.8</v>
       </c>
       <c r="E21">
-        <v>24.5</v>
+        <v>22.83</v>
       </c>
       <c r="F21">
-        <v>55.144607999999998</v>
+        <v>144.01900000000001</v>
       </c>
       <c r="G21">
-        <v>12.590981080000001</v>
+        <v>10.15329704</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22">
-        <v>33245</v>
+        <v>2234</v>
       </c>
       <c r="C22">
-        <v>0.80814439999999998</v>
+        <v>5.4305699999999998E-2</v>
       </c>
       <c r="D22">
-        <v>18686.400000000001</v>
+        <v>20765.400000000001</v>
       </c>
       <c r="E22">
-        <v>23.98</v>
+        <v>18.010000000000002</v>
       </c>
       <c r="F22">
-        <v>53.020954000000003</v>
+        <v>82.800003000000004</v>
       </c>
       <c r="G22">
-        <v>14.27296808</v>
+        <v>11.40276751</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23">
-        <v>3214</v>
+        <v>1739</v>
       </c>
       <c r="C23">
-        <v>7.8128299999999998E-2</v>
+        <v>4.2272900000000002E-2</v>
       </c>
       <c r="D23">
-        <v>6276.4</v>
+        <v>1705.8</v>
       </c>
       <c r="E23">
-        <v>21.01</v>
+        <v>16.25</v>
       </c>
       <c r="F23">
-        <v>75.694000000000003</v>
+        <v>237.19299000000001</v>
       </c>
       <c r="G23">
-        <v>9.4502071529999991</v>
+        <v>53.034999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24">
-        <v>116599</v>
+        <v>2627</v>
       </c>
       <c r="C24">
-        <v>2.8343758999999999</v>
+        <v>6.3859100000000002E-2</v>
       </c>
       <c r="D24">
-        <v>7906.6</v>
+        <v>6839.7</v>
       </c>
       <c r="E24">
-        <v>23.370000999999998</v>
+        <v>18.66</v>
       </c>
       <c r="F24">
-        <v>164.75800000000001</v>
+        <v>91.873001000000002</v>
       </c>
       <c r="G24">
-        <v>16.012018399999999</v>
+        <v>11.555999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
-        <v>540375</v>
+        <v>3214</v>
       </c>
       <c r="C25">
-        <v>13.135840999999999</v>
+        <v>7.8128299999999998E-2</v>
       </c>
       <c r="D25">
-        <v>36779.1</v>
+        <v>6276.4</v>
       </c>
       <c r="E25">
-        <v>25.32</v>
+        <v>21.01</v>
       </c>
       <c r="F25">
-        <v>70.530997999999997</v>
+        <v>75.694000000000003</v>
       </c>
       <c r="G25">
-        <v>5.3090000000000002</v>
+        <v>9.4502071529999991</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26">
-        <v>2120</v>
+        <v>116599</v>
       </c>
       <c r="C26">
-        <v>5.1534499999999997E-2</v>
+        <v>2.8343758999999999</v>
       </c>
       <c r="D26">
-        <v>20016.2</v>
+        <v>7906.6</v>
       </c>
       <c r="E26">
-        <v>21.440000999999999</v>
+        <v>23.370000999999998</v>
       </c>
       <c r="F26">
-        <v>74.647484000000006</v>
+        <v>164.75800000000001</v>
       </c>
       <c r="G26">
-        <v>21.555</v>
+        <v>16.012018399999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27">
-        <v>12472</v>
+        <v>2120</v>
       </c>
       <c r="C27">
-        <v>0.30317870000000002</v>
+        <v>5.1534499999999997E-2</v>
       </c>
       <c r="D27">
-        <v>22797.8</v>
+        <v>20016.2</v>
       </c>
       <c r="E27">
-        <v>21.709999</v>
+        <v>21.440000999999999</v>
       </c>
       <c r="F27">
-        <v>62.507747999999999</v>
+        <v>74.647484000000006</v>
       </c>
       <c r="G27">
-        <v>5.6364745440000004</v>
+        <v>21.555</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>12472</v>
+      </c>
+      <c r="C28">
+        <v>0.30317870000000002</v>
+      </c>
+      <c r="D28">
+        <v>22797.8</v>
+      </c>
+      <c r="E28">
+        <v>21.709999</v>
+      </c>
+      <c r="F28">
+        <v>62.507747999999999</v>
+      </c>
+      <c r="G28">
+        <v>5.6364745440000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>43299</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>1.0525445</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>15943.6</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>20.67</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>80</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>25.54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating all the things
</commit_message>
<xml_diff>
--- a/tables/Table1.xlsx
+++ b/tables/Table1.xlsx
@@ -1,137 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissoria/Documents/Research/us_international_ses/tables/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5A4926-8AC5-8742-BEDC-6B5EE0CAB203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="4980" windowWidth="25120" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Percent of Migrants</t>
-  </si>
-  <si>
-    <t>Life Expectancy at 60</t>
-  </si>
-  <si>
-    <t>Infant Mortality Rate (1950)</t>
-  </si>
-  <si>
-    <t>Infant Mortality Rate (2019)</t>
-  </si>
-  <si>
-    <t>Mexico and Carribean Countries</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Cuba</t>
-  </si>
-  <si>
-    <t>Dominican Republic</t>
-  </si>
-  <si>
-    <t>Puerto Rico</t>
-  </si>
-  <si>
-    <t>Central American Countries</t>
-  </si>
-  <si>
-    <t>Belize/British Honduras</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>El Salvador</t>
-  </si>
-  <si>
-    <t>Guatemala</t>
-  </si>
-  <si>
-    <t>Honduras</t>
-  </si>
-  <si>
-    <t>Nicaragua</t>
-  </si>
-  <si>
-    <t>Panama</t>
-  </si>
-  <si>
-    <t>South American Countries</t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Ecuador</t>
-  </si>
-  <si>
-    <t>Guyana/British Guiana</t>
-  </si>
-  <si>
-    <t>Haiti</t>
-  </si>
-  <si>
-    <t>Jamaica</t>
-  </si>
-  <si>
-    <t>Paraguay</t>
-  </si>
-  <si>
-    <t>Peru</t>
-  </si>
-  <si>
-    <t>Trinidad and Tobago</t>
-  </si>
-  <si>
-    <t>Uruguay</t>
-  </si>
-  <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
-    <t>GDP Per Capita</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,21 +63,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -231,7 +107,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -265,7 +141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -300,10 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -476,60 +350,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Percent of Migrants</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>GDP Per Capita</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Life Expectancy at 60</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Infant Mortality Rate (1950)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Infant Mortality Rate (2019)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Mexico and Carribean Countries</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
       </c>
       <c r="B3">
         <v>1809510</v>
       </c>
       <c r="C3">
-        <v>43.986924999999999</v>
+        <v>43.986925</v>
       </c>
       <c r="D3">
         <v>13790</v>
@@ -544,9 +426,11 @@
         <v>10.78765175</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
       </c>
       <c r="B4">
         <v>462503</v>
@@ -555,27 +439,29 @@
         <v>11.24287</v>
       </c>
       <c r="D4">
-        <v>9605.2999999999993</v>
+        <v>9605.299999999999</v>
       </c>
       <c r="E4">
         <v>21.57</v>
       </c>
       <c r="F4">
-        <v>87.121002000000004</v>
+        <v>87.121002</v>
       </c>
       <c r="G4">
-        <v>4.8892123959999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
+        <v>4.889212396</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
       </c>
       <c r="B5">
         <v>248511</v>
       </c>
       <c r="C5">
-        <v>6.0409917999999996</v>
+        <v>6.0409918</v>
       </c>
       <c r="D5">
         <v>10717.6</v>
@@ -587,18 +473,20 @@
         <v>63</v>
       </c>
       <c r="G5">
-        <v>4.1387709199999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
+        <v>4.13877092</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Puerto Rico</t>
+        </is>
       </c>
       <c r="B6">
         <v>540375</v>
       </c>
       <c r="C6">
-        <v>13.135840999999999</v>
+        <v>13.135841</v>
       </c>
       <c r="D6">
         <v>36779.1</v>
@@ -607,49 +495,55 @@
         <v>25.32</v>
       </c>
       <c r="F6">
-        <v>70.530997999999997</v>
+        <v>70.530998</v>
       </c>
       <c r="G6">
-        <v>5.3090000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
+        <v>5.309</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Central American Countries</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Belize/British Honduras</t>
+        </is>
       </c>
       <c r="B8">
         <v>1912</v>
       </c>
       <c r="C8">
-        <v>4.64783E-2</v>
+        <v>0.0464783</v>
       </c>
       <c r="D8">
         <v>7460</v>
       </c>
       <c r="E8">
-        <v>21.690000999999999</v>
+        <v>21.690001</v>
       </c>
       <c r="F8">
-        <v>89.337112000000005</v>
+        <v>89.337112</v>
       </c>
       <c r="G8">
         <v>12.42360178</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
       </c>
       <c r="B9">
         <v>20884</v>
       </c>
       <c r="C9">
-        <v>0.50766389999999995</v>
+        <v>0.5076638999999999</v>
       </c>
       <c r="D9">
         <v>16942</v>
@@ -658,21 +552,23 @@
         <v>24.52</v>
       </c>
       <c r="F9">
-        <v>80.935242000000002</v>
+        <v>80.935242</v>
       </c>
       <c r="G9">
-        <v>7.2910775140000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
+        <v>7.291077514</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
       </c>
       <c r="B10">
         <v>198955</v>
       </c>
       <c r="C10">
-        <v>4.8363472999999999</v>
+        <v>4.8363473</v>
       </c>
       <c r="D10">
         <v>5391.1</v>
@@ -681,21 +577,23 @@
         <v>22.01</v>
       </c>
       <c r="F10">
-        <v>78.046379000000002</v>
+        <v>78.046379</v>
       </c>
       <c r="G10">
         <v>14.05</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
       </c>
       <c r="B11">
         <v>99842</v>
       </c>
       <c r="C11">
-        <v>2.4270342999999999</v>
+        <v>2.4270343</v>
       </c>
       <c r="D11">
         <v>5762.8</v>
@@ -707,41 +605,45 @@
         <v>107</v>
       </c>
       <c r="G11">
-        <v>18.537905510000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>16</v>
+        <v>18.53790551</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
       </c>
       <c r="B12">
         <v>60125</v>
       </c>
       <c r="C12">
-        <v>1.4615636000000001</v>
+        <v>1.4615636</v>
       </c>
       <c r="D12">
         <v>3231.7</v>
       </c>
       <c r="E12">
-        <v>18.129999000000002</v>
+        <v>18.129999</v>
       </c>
       <c r="F12">
         <v>86</v>
       </c>
       <c r="G12">
-        <v>14.656000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>17</v>
+        <v>14.656</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Nicaragua</t>
+        </is>
       </c>
       <c r="B13">
         <v>60186</v>
       </c>
       <c r="C13">
-        <v>1.4630464999999999</v>
+        <v>1.4630465</v>
       </c>
       <c r="D13">
         <v>2612.9</v>
@@ -750,49 +652,55 @@
         <v>24.5</v>
       </c>
       <c r="F13">
-        <v>55.144607999999998</v>
+        <v>55.144608</v>
       </c>
       <c r="G13">
-        <v>12.590981080000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>18</v>
+        <v>12.59098108</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
       </c>
       <c r="B14">
         <v>33245</v>
       </c>
       <c r="C14">
-        <v>0.80814439999999998</v>
+        <v>0.8081444</v>
       </c>
       <c r="D14">
-        <v>18686.400000000001</v>
+        <v>18686.4</v>
       </c>
       <c r="E14">
         <v>23.98</v>
       </c>
       <c r="F14">
-        <v>53.020954000000003</v>
+        <v>53.020954</v>
       </c>
       <c r="G14">
         <v>14.27296808</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>20</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>South American Countries</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
       </c>
       <c r="B16">
         <v>48615</v>
       </c>
       <c r="C16">
-        <v>1.1817698999999999</v>
+        <v>1.1817699</v>
       </c>
       <c r="D16">
         <v>14187.5</v>
@@ -804,35 +712,39 @@
         <v>68</v>
       </c>
       <c r="G16">
-        <v>7.7482425089999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
+        <v>7.748242509</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Bolivia</t>
+        </is>
       </c>
       <c r="B17">
         <v>16749</v>
       </c>
       <c r="C17">
-        <v>0.40714729999999999</v>
+        <v>0.4071473</v>
       </c>
       <c r="D17">
         <v>3686.3</v>
       </c>
       <c r="E17">
-        <v>19.420000000000002</v>
+        <v>19.42</v>
       </c>
       <c r="F17">
         <v>182.161</v>
       </c>
       <c r="G17">
-        <v>28.826000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
+        <v>28.826</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
       </c>
       <c r="B18">
         <v>7814</v>
@@ -853,15 +765,17 @@
         <v>11.8134596</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>23</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
       </c>
       <c r="B19">
         <v>27920</v>
       </c>
       <c r="C19">
-        <v>0.67870030000000003</v>
+        <v>0.6787003</v>
       </c>
       <c r="D19">
         <v>17067.8</v>
@@ -873,41 +787,45 @@
         <v>139</v>
       </c>
       <c r="G19">
-        <v>6.5529999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>24</v>
+        <v>6.553</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Colombia</t>
+        </is>
       </c>
       <c r="B20">
         <v>194022</v>
       </c>
       <c r="C20">
-        <v>4.7164324999999998</v>
+        <v>4.7164325</v>
       </c>
       <c r="D20">
         <v>6947.4</v>
       </c>
       <c r="E20">
-        <v>22.690000999999999</v>
+        <v>22.690001</v>
       </c>
       <c r="F20">
-        <v>97.325325000000007</v>
+        <v>97.32532500000001</v>
       </c>
       <c r="G20">
-        <v>9.3586532479999995</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>25</v>
+        <v>9.358653248</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
       </c>
       <c r="B21">
         <v>91850</v>
       </c>
       <c r="C21">
-        <v>2.2327587000000002</v>
+        <v>2.2327587</v>
       </c>
       <c r="D21">
         <v>6609.8</v>
@@ -916,44 +834,48 @@
         <v>22.83</v>
       </c>
       <c r="F21">
-        <v>144.01900000000001</v>
+        <v>144.019</v>
       </c>
       <c r="G21">
         <v>10.15329704</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>26</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Guyana/British Guiana</t>
+        </is>
       </c>
       <c r="B22">
         <v>2234</v>
       </c>
       <c r="C22">
-        <v>5.4305699999999998E-2</v>
+        <v>0.0543057</v>
       </c>
       <c r="D22">
-        <v>20765.400000000001</v>
+        <v>20765.4</v>
       </c>
       <c r="E22">
-        <v>18.010000000000002</v>
+        <v>18.01</v>
       </c>
       <c r="F22">
-        <v>82.800003000000004</v>
+        <v>82.800003</v>
       </c>
       <c r="G22">
         <v>11.40276751</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>27</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
       </c>
       <c r="B23">
         <v>1739</v>
       </c>
       <c r="C23">
-        <v>4.2272900000000002E-2</v>
+        <v>0.0422729</v>
       </c>
       <c r="D23">
         <v>1705.8</v>
@@ -962,21 +884,23 @@
         <v>16.25</v>
       </c>
       <c r="F23">
-        <v>237.19299000000001</v>
+        <v>237.19299</v>
       </c>
       <c r="G23">
-        <v>53.034999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>28</v>
+        <v>53.035</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
       </c>
       <c r="B24">
         <v>2627</v>
       </c>
       <c r="C24">
-        <v>6.3859100000000002E-2</v>
+        <v>0.0638591</v>
       </c>
       <c r="D24">
         <v>6839.7</v>
@@ -985,21 +909,23 @@
         <v>18.66</v>
       </c>
       <c r="F24">
-        <v>91.873001000000002</v>
+        <v>91.873001</v>
       </c>
       <c r="G24">
-        <v>11.555999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>29</v>
+        <v>11.556</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Paraguay</t>
+        </is>
       </c>
       <c r="B25">
         <v>3214</v>
       </c>
       <c r="C25">
-        <v>7.8128299999999998E-2</v>
+        <v>0.0781283</v>
       </c>
       <c r="D25">
         <v>6276.4</v>
@@ -1008,67 +934,73 @@
         <v>21.01</v>
       </c>
       <c r="F25">
-        <v>75.694000000000003</v>
+        <v>75.694</v>
       </c>
       <c r="G25">
-        <v>9.4502071529999991</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>30</v>
+        <v>9.450207152999999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Peru</t>
+        </is>
       </c>
       <c r="B26">
         <v>116599</v>
       </c>
       <c r="C26">
-        <v>2.8343758999999999</v>
+        <v>2.8343759</v>
       </c>
       <c r="D26">
         <v>7906.6</v>
       </c>
       <c r="E26">
-        <v>23.370000999999998</v>
+        <v>23.370001</v>
       </c>
       <c r="F26">
-        <v>164.75800000000001</v>
+        <v>164.758</v>
       </c>
       <c r="G26">
-        <v>16.012018399999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>31</v>
+        <v>16.0120184</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
       </c>
       <c r="B27">
         <v>2120</v>
       </c>
       <c r="C27">
-        <v>5.1534499999999997E-2</v>
+        <v>0.0515345</v>
       </c>
       <c r="D27">
         <v>20016.2</v>
       </c>
       <c r="E27">
-        <v>21.440000999999999</v>
+        <v>21.440001</v>
       </c>
       <c r="F27">
-        <v>74.647484000000006</v>
+        <v>74.64748400000001</v>
       </c>
       <c r="G27">
         <v>21.555</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>32</v>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
       </c>
       <c r="B28">
         <v>12472</v>
       </c>
       <c r="C28">
-        <v>0.30317870000000002</v>
+        <v>0.3031787</v>
       </c>
       <c r="D28">
         <v>22797.8</v>
@@ -1077,15 +1009,17 @@
         <v>21.709999</v>
       </c>
       <c r="F28">
-        <v>62.507747999999999</v>
+        <v>62.507748</v>
       </c>
       <c r="G28">
-        <v>5.6364745440000004</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>33</v>
+        <v>5.636474544</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Venezuela</t>
+        </is>
       </c>
       <c r="B29">
         <v>43299</v>

</xml_diff>